<commit_message>
updated yumbe users sheet
</commit_message>
<xml_diff>
--- a/sheets/GetInYumbeUsers.xlsx
+++ b/sheets/GetInYumbeUsers.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$F$1:$J$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$F$1:$J$44</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$F$1:$J$44</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$F$1:$J$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -209,7 +209,7 @@
     <t xml:space="preserve">Rukia</t>
   </si>
   <si>
-    <t xml:space="preserve">mrukia</t>
+    <t xml:space="preserve">maliko</t>
   </si>
   <si>
     <t xml:space="preserve">Bolli</t>
@@ -839,15 +839,15 @@
   </sheetPr>
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="23.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.03"/>
@@ -7367,7 +7367,7 @@
       <c r="I999" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="F1:J1"/>
+  <autoFilter ref="F1:J44"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>